<commit_message>
Another Modi by Abd
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Sam </t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>on</t>
+  </si>
+  <si>
+    <t>ejr;lkwjlkw`kjkejg</t>
+  </si>
+  <si>
+    <t>kj;lknds</t>
+  </si>
+  <si>
+    <t>n;lkngdlkndlkgn;lkdg</t>
   </si>
 </sst>
 </file>
@@ -352,7 +361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -360,15 +369,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H2"/>
+  <dimension ref="A2:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -392,6 +401,15 @@
       </c>
       <c r="H2" t="s">
         <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>